<commit_message>
[Wordpress_Review Data] 엡마스터도구, SNS 연동(페이스북) sheet 추가
</commit_message>
<xml_diff>
--- a/Wordpress_Review Data.xlsx
+++ b/Wordpress_Review Data.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="WP 구조" sheetId="6" r:id="rId1"/>
     <sheet name="PHP 설명" sheetId="7" r:id="rId2"/>
     <sheet name="Link" sheetId="8" r:id="rId3"/>
     <sheet name="Tip" sheetId="9" r:id="rId4"/>
+    <sheet name="웹마스터도구" sheetId="10" r:id="rId5"/>
+    <sheet name="SNS 연동" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'SNS 연동'!$A$1:$O$192</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">웹마스터도구!$A$1:$O$106</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
   <si>
     <t>theme에서 사용 여부를 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -319,12 +325,184 @@
     <t>수동으로 일일히 삭제하는 방법을 사용하지는 않으며 wp clean up 이라는 플러그인을 사용합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>검색엔진에서 제공하는 도구로 검색노출이 잘 될 수 있도록 검색엔지과 동기화시켜주는 tool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹마스터도구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구글 웹마스터도구 사이트를 방문하여 로그인을 한 이후에 접속을 하게 되면 아래와 같은 화면이 나타납니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹사이트에 자신의 site URL를 등록한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 구글에서 제공하는 HTML file을 Donwload 받는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. FTP program을 이용하여 사이트 root folder에 HTML file를 upload한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 아래 link를 웹브라우저에 입력하여 해당 페이지가 열리는지 확인한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 로봇이 아닙니다를 check후 확인을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색노출이 필요한 사이트는 아래 검색엔진들에 모두 등록한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹마스터도구 페이지에 접속한후 네이버 ID로 로그인 후 사이트 추가를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사이트 URL 입력 후 확인을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTML 파일 업로드 방식은 구글과 동일함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTML 태그는 홈페이지 &lt;head&gt; 센션에 네이버에서 제공하는 메타태그를 추가하는 방식이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 네이버 - http://webmastertool.naver.com/board/main.naver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. google - https://www.google.com/webmasters/tools/home?hl=ko</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관련 플러그인은 검색엔진의 웹서치 로봇의 방문을 기다리지 않고 다이렉트로 노출등록해준다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNS 연동 - 워드프레스 Post의 자동발행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스에서 발행되는 블로그 포스트를 자동으로 SNS에도 발행함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 페이스북</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API ( Application Programming Interface)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">응용프로그램의 인터페이스를 의미하며, 파일, 문자 , 제어 등을 위한 인터페이스가 제공됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">보통 SNS의 앱ID, 앱 시크릿코드, API 키의 정보가 필요함. 아무나 내 페이스북을 사용하지 못하도록 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">보안차원에서 앱ID, 시크릿코드, API키등이 일치해야 페이스북을 사용할수 있도록 제한하는 것입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">로그인 상태에서 먼저 페이스북 개발자사이트에 접속하여 개발자 등록을 마칩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developers.facebook.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ilovehwa0311</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발자 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발자 화면에서 [시작하기] 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Popup 창에서 '예'를 선택 후 등록 버튼을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[앱 ID 만들기] 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래 정보들을 입력하고, [앱 ID 만들기] 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보안 문자를 입력 후 [제출]를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록 완료 후 대시보드를 확인하면, 아래와 같이 API 버전, 앱 ID, 앱 시크릿 코드를 확인할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앱 시크릿 코드는 [보기] 버튼을 눌러 코드값을 확인 할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01062968317</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왼쪽 메뉴에서 [설정]을 선택하고, 앱 도메인을 입력 후, 하단 [플렛폼 추가]를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플렛폼 선택 창에서 웹사이트를 더블 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앱 도메인에 www가 있는 주소와 없는 주소를 모두 입력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하단의 사이트 URL에 사이트 주소를 입력하고 변경 내용을 저장한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앱 검수 메뉴에서 모든 권한을 [예]로 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 설정이 완료 되었으며, 대시보드의 아래 정보를 이용하여 SNS 플러그인에서 등록하면 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +542,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -397,13 +584,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -414,6 +604,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -6787,6 +6980,2085 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="그룹 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="666750" y="1828800"/>
+          <a:ext cx="7324725" cy="3905250"/>
+          <a:chOff x="1219200" y="1333500"/>
+          <a:chExt cx="9753600" cy="5029200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="그림 4"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1219200" y="1333500"/>
+            <a:ext cx="9753600" cy="5029200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2876550" y="2476500"/>
+            <a:ext cx="6543675" cy="523875"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>141262</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="그룹 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="619125" y="6838950"/>
+          <a:ext cx="7219950" cy="4246537"/>
+          <a:chOff x="514350" y="6896100"/>
+          <a:chExt cx="8210550" cy="4829175"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="그림 8"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="514350" y="6896100"/>
+            <a:ext cx="8210550" cy="4829175"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="8543925"/>
+            <a:ext cx="7800975" cy="1228725"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>565548</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="16" name="그룹 15"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="666751" y="11972925"/>
+          <a:ext cx="2861072" cy="2543175"/>
+          <a:chOff x="666751" y="11591925"/>
+          <a:chExt cx="3333750" cy="2963333"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="14" name="그림 13"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="666751" y="11591925"/>
+            <a:ext cx="3333750" cy="2963333"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="모서리가 둥근 직사각형 14"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="13068300"/>
+            <a:ext cx="1362075" cy="1209675"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>42915</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>345559</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="그룹 19"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3686175" y="11825340"/>
+          <a:ext cx="4422259" cy="2652660"/>
+          <a:chOff x="733425" y="14959065"/>
+          <a:chExt cx="6391275" cy="3833760"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="18" name="그림 17"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="733425" y="14959065"/>
+            <a:ext cx="6391275" cy="3833760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 18"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2152651" y="16764000"/>
+            <a:ext cx="4743450" cy="600075"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>633390</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="그룹 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="676275" y="15411450"/>
+          <a:ext cx="7034190" cy="6191250"/>
+          <a:chOff x="676275" y="15363825"/>
+          <a:chExt cx="7034190" cy="6191250"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="22" name="그림 21"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="676275" y="15363825"/>
+            <a:ext cx="7034190" cy="6191250"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="모서리가 둥근 직사각형 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2105025" y="16678275"/>
+            <a:ext cx="5381625" cy="1238250"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="모서리가 둥근 직사각형 23"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2076450" y="18116550"/>
+            <a:ext cx="5400675" cy="428625"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>140634</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>50427</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>86369</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="그룹 8"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1016934" y="4498602"/>
+          <a:ext cx="3998819" cy="1712342"/>
+          <a:chOff x="1037105" y="5205133"/>
+          <a:chExt cx="3994336" cy="1739236"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="그림 4"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1037105" y="5205133"/>
+            <a:ext cx="3994336" cy="1739236"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4258237" y="5827058"/>
+            <a:ext cx="705970" cy="336177"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4403912" y="6539752"/>
+            <a:ext cx="600636" cy="336177"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>103655</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>35860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63438</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="11" name="그룹 10"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="979955" y="3017185"/>
+          <a:ext cx="6599703" cy="1075328"/>
+          <a:chOff x="1000126" y="3700184"/>
+          <a:chExt cx="6586256" cy="1092136"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1000126" y="3700184"/>
+            <a:ext cx="6586256" cy="1092136"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6703360" y="3711389"/>
+            <a:ext cx="647699" cy="289112"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>58382</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="그룹 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1019175" y="6591300"/>
+          <a:ext cx="4010025" cy="1268057"/>
+          <a:chOff x="1019175" y="7219950"/>
+          <a:chExt cx="4010025" cy="1268057"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="13" name="그림 12"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1019175" y="7219950"/>
+            <a:ext cx="4010025" cy="1268057"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="모서리가 둥근 직사각형 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4091829" y="8097370"/>
+            <a:ext cx="823071" cy="303680"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>4112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="그림 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1019175" y="8286750"/>
+          <a:ext cx="4010025" cy="2032937"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>121513</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="그림 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1028701" y="11039475"/>
+          <a:ext cx="4019550" cy="1912213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="그룹 34"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1009651" y="13535026"/>
+          <a:ext cx="6962774" cy="3371849"/>
+          <a:chOff x="1009651" y="13535026"/>
+          <a:chExt cx="6962774" cy="3371849"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="27" name="그룹 26"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1009651" y="13535026"/>
+            <a:ext cx="6962774" cy="2573768"/>
+            <a:chOff x="1009651" y="13535025"/>
+            <a:chExt cx="7137690" cy="2638425"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="그림 23"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="1009651" y="13535025"/>
+              <a:ext cx="7137690" cy="2638425"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 24"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3971367" y="14636002"/>
+              <a:ext cx="3305734" cy="832598"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="26" name="모서리가 둥근 직사각형 25"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6876491" y="15188452"/>
+              <a:ext cx="362509" cy="251573"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="33" name="그룹 32"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2209800" y="15354300"/>
+            <a:ext cx="5715000" cy="1552575"/>
+            <a:chOff x="2209800" y="15354300"/>
+            <a:chExt cx="5715000" cy="1552575"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="29" name="그림 28"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="2209800" y="16306800"/>
+              <a:ext cx="5715000" cy="600075"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="31" name="직선 화살표 연결선 30"/>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="3276600" y="15354300"/>
+              <a:ext cx="3524250" cy="990600"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>87249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>96139</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="41" name="그룹 40"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="971550" y="17317974"/>
+          <a:ext cx="7048500" cy="3571240"/>
+          <a:chOff x="971550" y="17317974"/>
+          <a:chExt cx="7048500" cy="3571240"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="37" name="그림 36"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="971550" y="17317974"/>
+            <a:ext cx="7048500" cy="3571240"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="40" name="그룹 39"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="3266516" y="18503152"/>
+            <a:ext cx="4696384" cy="2242298"/>
+            <a:chOff x="3266516" y="18503152"/>
+            <a:chExt cx="4696384" cy="2242298"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="38" name="모서리가 둥근 직사각형 37"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3390341" y="18503152"/>
+              <a:ext cx="2210359" cy="413498"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="39" name="모서리가 둥근 직사각형 38"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3266516" y="20427202"/>
+              <a:ext cx="4696384" cy="318248"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>92010</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="45" name="그룹 44"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1000125" y="21469350"/>
+          <a:ext cx="4391025" cy="2768535"/>
+          <a:chOff x="1000125" y="21469350"/>
+          <a:chExt cx="4391025" cy="2768535"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="43" name="그림 42"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1000125" y="21469350"/>
+            <a:ext cx="4391025" cy="2768535"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="모서리가 둥근 직사각형 43"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2218767" y="22027401"/>
+            <a:ext cx="810184" cy="689723"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>35780</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="50" name="그룹 49"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="971550" y="24860251"/>
+          <a:ext cx="4981575" cy="4560154"/>
+          <a:chOff x="971550" y="24841201"/>
+          <a:chExt cx="4981575" cy="4560154"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="47" name="그림 46"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="971550" y="24841201"/>
+            <a:ext cx="4981575" cy="4560154"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="48" name="모서리가 둥근 직사각형 47"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1066241" y="25913601"/>
+            <a:ext cx="2381809" cy="442073"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="49" name="모서리가 둥근 직사각형 48"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1028700" y="28437726"/>
+            <a:ext cx="4829175" cy="442073"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>87474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="그림 51"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="933450" y="34737675"/>
+          <a:ext cx="6772275" cy="2487774"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>38573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="그림 53"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="971551" y="29813250"/>
+          <a:ext cx="5467349" cy="4429598"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>208991</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>24652</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="모서리가 둥근 직사각형 54"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1085291" y="30247477"/>
+          <a:ext cx="3772459" cy="337298"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189941</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>81802</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="모서리가 둥근 직사각형 55"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066241" y="32819227"/>
+          <a:ext cx="5048809" cy="1346948"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -6830,7 +9102,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6865,7 +9137,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7374,8 +9646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7544,4 +9816,267 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D72"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T56" sqref="T56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.5" customWidth="1"/>
+    <col min="3" max="3" width="2.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="4.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N165"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N190" sqref="N190"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.875" customWidth="1"/>
+    <col min="2" max="3" width="2.875" style="6" customWidth="1"/>
+    <col min="4" max="5" width="2.875" customWidth="1"/>
+    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C9" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E102" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E117" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E118" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D142" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D165" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId2"/>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="101" max="14" man="1"/>
+    <brk id="141" max="14" man="1"/>
+  </rowBreaks>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Wordpress_Review Data] 카페24 서버 구축 manual 추가
</commit_message>
<xml_diff>
--- a/Wordpress_Review Data.xlsx
+++ b/Wordpress_Review Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WP 구조" sheetId="6" r:id="rId1"/>
@@ -13,8 +13,10 @@
     <sheet name="Tip" sheetId="9" r:id="rId4"/>
     <sheet name="웹마스터도구" sheetId="10" r:id="rId5"/>
     <sheet name="SNS 연동" sheetId="11" r:id="rId6"/>
+    <sheet name="Cafe24" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Cafe24!$A$1:$O$140</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'SNS 연동'!$A$1:$O$192</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">웹마스터도구!$A$1:$O$106</definedName>
   </definedNames>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="131">
   <si>
     <t>theme에서 사용 여부를 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -495,6 +497,74 @@
   </si>
   <si>
     <t>모든 설정이 완료 되었으며, 대시보드의 아래 정보를 이용하여 SNS 플러그인에서 등록하면 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카페 24에서 PHP 버전 변경하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">사이트 속도 향상을 위해 PHP 7.0으로 변경하는 것이 좋습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 7.0으로 변경할 경우 데이터, DB 모두 초기화되므로 반드시 백업을 받아놓고 시작하시기 바랍니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러 아이디가 있는 경우 상단의 “내가 신청한 아이디 목록”에서 해당 아이디 선택 &gt; 연장/변경/추가옵션 &gt; 변경신청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우커머스의 경우 PHP v5.6, MySQL v5.6 이상이 recommand 사양임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 후 계정관리&gt;백업받기/올리기를 선택하고, DB 백업받기를 선태하면 아래와 같은 화면이 나옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백업받기 선택하면 백업파일경로로 백업이 진행됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 7.0을 선택하고 변경신청을 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FTP 비번을 입력하고 아래와 같이 check box를 선택 후 변경 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래와 같은 재확인 box가 나오며, 예를 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. DB 백업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. cafe24 Login후 나의 서비스관리 연장/변경/추가옵션의 변경신청 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. DB 백업 복원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정관리의 DATA&amp;DB복원/백업 을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB / 복원하기를 선택 후 실행을 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Café24 호스팅 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP 사용을 위해서 아래와 같은 서버 환경으로 구매한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9059,6 +9129,1068 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>122702</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="그림 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2352675" y="2019300"/>
+          <a:ext cx="5638800" cy="875177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="그림 48"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="962025" y="15830550"/>
+          <a:ext cx="4391025" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="53" name="그룹 52"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="771525" y="7305675"/>
+          <a:ext cx="1495425" cy="1276350"/>
+          <a:chOff x="771525" y="2019300"/>
+          <a:chExt cx="1495425" cy="1276350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="51" name="그림 50"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="771525" y="2019300"/>
+            <a:ext cx="1495425" cy="1276350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="52" name="모서리가 둥근 직사각형 51"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="771525" y="2295525"/>
+            <a:ext cx="1104900" cy="200025"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="56" name="그룹 55"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="933450" y="9134475"/>
+          <a:ext cx="2038350" cy="1524000"/>
+          <a:chOff x="933450" y="3848100"/>
+          <a:chExt cx="2038350" cy="1524000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="39" name="그림 38"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="933450" y="3848100"/>
+            <a:ext cx="2038350" cy="1524000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="54" name="모서리가 둥근 직사각형 53"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1019175" y="5048250"/>
+            <a:ext cx="1866900" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="57" name="그룹 56"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3429000" y="9163050"/>
+          <a:ext cx="1447800" cy="2314575"/>
+          <a:chOff x="3429000" y="3876675"/>
+          <a:chExt cx="1447800" cy="2314575"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="41" name="그림 40"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="3429000" y="3876675"/>
+            <a:ext cx="1447800" cy="2314575"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="55" name="모서리가 둥근 직사각형 54"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3457575" y="4657725"/>
+            <a:ext cx="1304925" cy="190500"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>18357</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="60" name="그룹 59"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="923925" y="11887200"/>
+          <a:ext cx="7010400" cy="3314007"/>
+          <a:chOff x="923925" y="6600825"/>
+          <a:chExt cx="7010400" cy="3314007"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="45" name="그림 44"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="923925" y="6600825"/>
+            <a:ext cx="7010400" cy="3314007"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="58" name="모서리가 둥근 직사각형 57"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1095375" y="8562975"/>
+            <a:ext cx="676275" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="59" name="모서리가 둥근 직사각형 58"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6667500" y="9429749"/>
+            <a:ext cx="1123950" cy="371475"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>140438</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="63" name="그룹 62"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="962025" y="15878175"/>
+          <a:ext cx="6924675" cy="4683863"/>
+          <a:chOff x="962025" y="10591800"/>
+          <a:chExt cx="6924675" cy="4683863"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="47" name="그림 46"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="962025" y="10591800"/>
+            <a:ext cx="6924675" cy="4683863"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="61" name="모서리가 둥근 직사각형 60"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2190750" y="12001500"/>
+            <a:ext cx="1419225" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="62" name="모서리가 둥근 직사각형 61"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5248275" y="14544675"/>
+            <a:ext cx="2590800" cy="276225"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="67" name="그룹 66"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="904875" y="23622000"/>
+          <a:ext cx="1476375" cy="1266825"/>
+          <a:chOff x="904875" y="18335625"/>
+          <a:chExt cx="1476375" cy="1266825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="66" name="그림 65"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="914400" y="18335625"/>
+            <a:ext cx="1466850" cy="1266825"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="64" name="모서리가 둥근 직사각형 63"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="904875" y="18783300"/>
+            <a:ext cx="1438275" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>10631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="그림 68"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="20269200"/>
+          <a:ext cx="7000875" cy="3468206"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="그림 70"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="733425" y="742950"/>
+          <a:ext cx="5010150" cy="2819400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="그림 72"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="723900" y="676275"/>
+          <a:ext cx="6496050" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -9102,7 +10234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9137,7 +10269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9348,7 +10480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
@@ -9925,7 +11057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N165"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="N190" sqref="N190"/>
     </sheetView>
   </sheetViews>
@@ -10079,4 +11211,128 @@
   </rowBreaks>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:N120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U48" sqref="U48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.875" customWidth="1"/>
+    <col min="2" max="3" width="2.875" style="6" customWidth="1"/>
+    <col min="4" max="5" width="2.875" customWidth="1"/>
+    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B27" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C42" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D47" s="4"/>
+      <c r="N47" s="8"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C111" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="5" manualBreakCount="5">
+    <brk id="26" max="14" man="1"/>
+    <brk id="74" max="14" man="1"/>
+    <brk id="110" max="14" man="1"/>
+    <brk id="140" max="14" man="1"/>
+    <brk id="184" max="14" man="1"/>
+  </rowBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Wordpress_Review Data] 카페24 WP 설치 및 테마 설치 메뉴얼 추가
</commit_message>
<xml_diff>
--- a/Wordpress_Review Data.xlsx
+++ b/Wordpress_Review Data.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Cafe24" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">Cafe24!$A$1:$O$140</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Cafe24!$A$1:$O$204</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'SNS 연동'!$A$1:$O$192</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">웹마스터도구!$A$1:$O$106</definedName>
   </definedNames>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="138">
   <si>
     <t>theme에서 사용 여부를 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -565,6 +565,34 @@
   </si>
   <si>
     <t>WP 사용을 위해서 아래와 같은 서버 환경으로 구매한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카페 24에서 WP 설치 및 테마 설치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의서비스관리 선택 후, 프로그램 자동설치를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스를 선택하고 설치하기를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP 설치 - WP만 설치되고, 테마도 같이 설치시에는 테마 설치에서 WP까지 같이 설치하는 것이 좋다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WP 테마 설치 - 테마에 맞춰 WP도 같이 설치되므로, 테마에 optimize가 되어 설치된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의서비스관리 선택 후, 워드프레스 테마 설치를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스 테마 선택에서 원하는 테마에 마우스를 올리면 아래와 같이 설치하기 메뉴가 활성화 됨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -10188,6 +10216,411 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>88988</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="그룹 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="895350" y="32042100"/>
+          <a:ext cx="7200900" cy="4441913"/>
+          <a:chOff x="704850" y="29908500"/>
+          <a:chExt cx="7200900" cy="4441913"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="28" name="그림 27"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="733425" y="29908500"/>
+            <a:ext cx="7172325" cy="4441913"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="모서리가 둥근 직사각형 28"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="704850" y="31946850"/>
+            <a:ext cx="1152525" cy="180975"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="31" name="그룹 30"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="904875" y="30146625"/>
+          <a:ext cx="2038350" cy="1524000"/>
+          <a:chOff x="933450" y="3848100"/>
+          <a:chExt cx="2038350" cy="1524000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="32" name="그림 31"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="933450" y="3848100"/>
+            <a:ext cx="2038350" cy="1524000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="모서리가 둥근 직사각형 32"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1019175" y="5048250"/>
+            <a:ext cx="1866900" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>80182</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="그룹 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="952500" y="37566600"/>
+          <a:ext cx="7124700" cy="4776007"/>
+          <a:chOff x="914400" y="37547550"/>
+          <a:chExt cx="7124700" cy="4776007"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="3" name="그룹 2"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="914400" y="37547550"/>
+            <a:ext cx="7124700" cy="4776007"/>
+            <a:chOff x="914400" y="37547550"/>
+            <a:chExt cx="7124700" cy="4776007"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="35" name="그림 34"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="923925" y="37566601"/>
+              <a:ext cx="7115175" cy="4756956"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="36" name="모서리가 둥근 직사각형 35"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="914400" y="37547550"/>
+              <a:ext cx="1343025" cy="209550"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="모서리가 둥근 직사각형 37"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5305425" y="40405050"/>
+            <a:ext cx="600075" cy="361950"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11218,10 +11651,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:N120"/>
+  <dimension ref="B2:N178"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A176" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R192" sqref="R192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11322,6 +11755,41 @@
         <v>128</v>
       </c>
     </row>
+    <row r="141" spans="2:4" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B141" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C142" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D143" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D152" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C176" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D177" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D178" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11331,7 +11799,7 @@
     <brk id="74" max="14" man="1"/>
     <brk id="110" max="14" man="1"/>
     <brk id="140" max="14" man="1"/>
-    <brk id="184" max="14" man="1"/>
+    <brk id="175" max="14" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
[Wordpress_Review Data] WP 업로드 파일 형식 추가 방법
</commit_message>
<xml_diff>
--- a/Wordpress_Review Data.xlsx
+++ b/Wordpress_Review Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WP 구조" sheetId="6" r:id="rId1"/>
@@ -14,10 +14,12 @@
     <sheet name="웹마스터도구" sheetId="10" r:id="rId5"/>
     <sheet name="SNS 연동" sheetId="11" r:id="rId6"/>
     <sheet name="Cafe24" sheetId="12" r:id="rId7"/>
+    <sheet name="WP 설정" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Cafe24!$A$1:$O$204</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'SNS 연동'!$A$1:$O$192</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'WP 설정'!$A$1:$P$48</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">웹마스터도구!$A$1:$O$106</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
   <si>
     <t>theme에서 사용 여부를 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -593,6 +595,58 @@
   </si>
   <si>
     <t>워드프레스 테마 선택에서 원하는 테마에 마우스를 올리면 아래와 같이 설치하기 메뉴가 활성화 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 업로드 파일 형식 추가 지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스는 지원하지 못하는 형식의 파일은 업로드가 안됨.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이를 추가하기 위해서는 Plug-in이나 function.php에 code를 추가해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ko.wordpress.org/plugins/wp-add-mime-types/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아래 link의 WP Add Mime Types 플러그인 설치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Plug-in 사용 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>“관리자화면-설정-Mime Type Settings” 화면으로 가서 화면의 하단 “Add Values” 에 다음과 같이 입력, 저장.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력한 값의 앞 단어는 원하는 파일의 확장자 이고, 뒤 문구는 해당 파일의 mime type 입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) function.php 수정 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 테마 차일드 테마의 functions.php 파일의 하단에 아래의 코드를 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 사이트의 wp-config.php 파일의 하단에 다음 코드를 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>define('ALLOW_UNFILTERED_UPLOADS', true );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 설정은 관리자에게만 해당되므로, 다른 사용자(에디터,저자 등)는 사용 할 수 없습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -10624,6 +10678,121 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>36636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>564173</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>185459</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="908538" y="1948963"/>
+          <a:ext cx="6704135" cy="3336034"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="942975" y="6115050"/>
+          <a:ext cx="3810000" cy="1895475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -11653,8 +11822,8 @@
   </sheetPr>
   <dimension ref="B2:N178"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A176" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R192" sqref="R192"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11803,4 +11972,93 @@
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="2.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>